<commit_message>
updated notebooks and re-exported results
</commit_message>
<xml_diff>
--- a/experiments/2022_scientific_reports/results/statistics/stats_cortisol_features.xlsx
+++ b/experiments/2022_scientific_reports/results/statistics/stats_cortisol_features.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="parameter" sheetId="1" r:id="rId1"/>
     <sheet name="normality" sheetId="2" r:id="rId2"/>
-    <sheet name="pairwise_ttests" sheetId="3" r:id="rId3"/>
+    <sheet name="pairwise_tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -108,7 +108,7 @@
     <t>two-sided</t>
   </si>
   <si>
-    <t>Pairwise t-Tests</t>
+    <t>Pairwise Tests</t>
   </si>
 </sst>
 </file>

</xml_diff>